<commit_message>
ingresan a One Drive
</commit_message>
<xml_diff>
--- a/asset/Control GESPRO.xlsx
+++ b/asset/Control GESPRO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="152">
   <si>
     <t>Sección</t>
   </si>
@@ -472,6 +472,15 @@
   </si>
   <si>
     <t>recomennd</t>
+  </si>
+  <si>
+    <t>iiiciclo</t>
+  </si>
+  <si>
+    <t>diversifi</t>
+  </si>
+  <si>
+    <t>mp3</t>
   </si>
 </sst>
 </file>
@@ -999,7 +1008,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1170,9 +1179,6 @@
     <xf numFmtId="0" fontId="4" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1180,6 +1186,13 @@
     <xf numFmtId="0" fontId="9" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1252,10 +1265,9 @@
     <xf numFmtId="0" fontId="9" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1597,14 +1609,14 @@
       <c r="L2" s="22"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G3" s="108" t="s">
+      <c r="G3" s="110" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="109"/>
-      <c r="I3" s="109"/>
-      <c r="J3" s="109"/>
-      <c r="K3" s="109"/>
-      <c r="L3" s="110"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="112"/>
     </row>
     <row r="4" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1648,10 +1660,10 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="116" t="s">
+      <c r="B5" s="118" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1676,13 +1688,13 @@
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="102" t="s">
+      <c r="M5" s="104" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="106"/>
-      <c r="B6" s="117"/>
+      <c r="A6" s="108"/>
+      <c r="B6" s="119"/>
       <c r="C6" s="8" t="s">
         <v>6</v>
       </c>
@@ -1705,11 +1717,11 @@
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="103"/>
+      <c r="M6" s="105"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="106"/>
-      <c r="B7" s="117"/>
+      <c r="A7" s="108"/>
+      <c r="B7" s="119"/>
       <c r="C7" s="8" t="s">
         <v>7</v>
       </c>
@@ -1732,11 +1744,11 @@
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="103"/>
+      <c r="M7" s="105"/>
     </row>
     <row r="8" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="106"/>
-      <c r="B8" s="117"/>
+      <c r="A8" s="108"/>
+      <c r="B8" s="119"/>
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
@@ -1759,11 +1771,11 @@
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="103"/>
+      <c r="M8" s="105"/>
     </row>
     <row r="9" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="106"/>
-      <c r="B9" s="117"/>
+      <c r="A9" s="108"/>
+      <c r="B9" s="119"/>
       <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
@@ -1786,11 +1798,11 @@
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="103"/>
+      <c r="M9" s="105"/>
     </row>
     <row r="10" spans="1:13" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="106"/>
-      <c r="B10" s="117"/>
+      <c r="A10" s="108"/>
+      <c r="B10" s="119"/>
       <c r="C10" s="8" t="s">
         <v>10</v>
       </c>
@@ -1813,11 +1825,11 @@
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="103"/>
+      <c r="M10" s="105"/>
     </row>
     <row r="11" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="106"/>
-      <c r="B11" s="117"/>
+      <c r="A11" s="108"/>
+      <c r="B11" s="119"/>
       <c r="C11" s="8" t="s">
         <v>11</v>
       </c>
@@ -1840,11 +1852,11 @@
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="103"/>
+      <c r="M11" s="105"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="106"/>
-      <c r="B12" s="117"/>
+      <c r="A12" s="108"/>
+      <c r="B12" s="119"/>
       <c r="C12" s="8" t="s">
         <v>12</v>
       </c>
@@ -1867,11 +1879,11 @@
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="103"/>
+      <c r="M12" s="105"/>
     </row>
     <row r="13" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="106"/>
-      <c r="B13" s="117"/>
+      <c r="A13" s="108"/>
+      <c r="B13" s="119"/>
       <c r="C13" s="8" t="s">
         <v>13</v>
       </c>
@@ -1894,18 +1906,18 @@
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="103"/>
+      <c r="M13" s="105"/>
     </row>
     <row r="14" spans="1:13" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="106"/>
-      <c r="B14" s="117"/>
-      <c r="C14" s="111" t="s">
+      <c r="A14" s="108"/>
+      <c r="B14" s="119"/>
+      <c r="C14" s="113" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="9">
         <v>31</v>
       </c>
-      <c r="E14" s="114" t="s">
+      <c r="E14" s="116" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="13" t="s">
@@ -1925,16 +1937,16 @@
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="103"/>
+      <c r="M14" s="105"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="106"/>
-      <c r="B15" s="117"/>
-      <c r="C15" s="112"/>
+      <c r="A15" s="108"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="114"/>
       <c r="D15" s="10">
         <v>31</v>
       </c>
-      <c r="E15" s="119"/>
+      <c r="E15" s="121"/>
       <c r="F15" s="12" t="s">
         <v>14</v>
       </c>
@@ -1952,16 +1964,16 @@
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="103"/>
+      <c r="M15" s="105"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="106"/>
-      <c r="B16" s="117"/>
-      <c r="C16" s="112"/>
+      <c r="A16" s="108"/>
+      <c r="B16" s="119"/>
+      <c r="C16" s="114"/>
       <c r="D16" s="10">
         <v>31</v>
       </c>
-      <c r="E16" s="115"/>
+      <c r="E16" s="117"/>
       <c r="F16" s="12" t="s">
         <v>16</v>
       </c>
@@ -1979,16 +1991,16 @@
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="103"/>
+      <c r="M16" s="105"/>
     </row>
     <row r="17" spans="1:15" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="106"/>
-      <c r="B17" s="117"/>
-      <c r="C17" s="112"/>
+      <c r="A17" s="108"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="114"/>
       <c r="D17" s="10">
         <v>31</v>
       </c>
-      <c r="E17" s="114" t="s">
+      <c r="E17" s="116" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="11" t="s">
@@ -2008,16 +2020,16 @@
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="103"/>
+      <c r="M17" s="105"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="106"/>
-      <c r="B18" s="117"/>
-      <c r="C18" s="112"/>
+      <c r="A18" s="108"/>
+      <c r="B18" s="119"/>
+      <c r="C18" s="114"/>
       <c r="D18" s="10">
         <v>31</v>
       </c>
-      <c r="E18" s="119"/>
+      <c r="E18" s="121"/>
       <c r="F18" s="12" t="s">
         <v>14</v>
       </c>
@@ -2035,16 +2047,16 @@
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="103"/>
+      <c r="M18" s="105"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="106"/>
-      <c r="B19" s="117"/>
-      <c r="C19" s="113"/>
+      <c r="A19" s="108"/>
+      <c r="B19" s="119"/>
+      <c r="C19" s="115"/>
       <c r="D19" s="10">
         <v>31</v>
       </c>
-      <c r="E19" s="115"/>
+      <c r="E19" s="117"/>
       <c r="F19" s="12" t="s">
         <v>16</v>
       </c>
@@ -2062,12 +2074,12 @@
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="103"/>
+      <c r="M19" s="105"/>
     </row>
     <row r="20" spans="1:15" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="106"/>
-      <c r="B20" s="117"/>
-      <c r="C20" s="111" t="s">
+      <c r="A20" s="108"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="113" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="9">
@@ -2091,12 +2103,12 @@
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="103"/>
+      <c r="M20" s="105"/>
     </row>
     <row r="21" spans="1:15" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="106"/>
-      <c r="B21" s="117"/>
-      <c r="C21" s="112"/>
+      <c r="A21" s="108"/>
+      <c r="B21" s="119"/>
+      <c r="C21" s="114"/>
       <c r="D21" s="10">
         <v>29</v>
       </c>
@@ -2118,11 +2130,11 @@
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="103"/>
+      <c r="M21" s="105"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="106"/>
-      <c r="B22" s="117"/>
+      <c r="A22" s="108"/>
+      <c r="B22" s="119"/>
       <c r="C22" s="7" t="s">
         <v>19</v>
       </c>
@@ -2145,11 +2157,11 @@
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="103"/>
+      <c r="M22" s="105"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="107"/>
-      <c r="B23" s="118"/>
+      <c r="A23" s="109"/>
+      <c r="B23" s="120"/>
       <c r="C23" s="8" t="s">
         <v>16</v>
       </c>
@@ -2172,7 +2184,7 @@
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="104"/>
+      <c r="M23" s="106"/>
     </row>
     <row r="24" spans="1:15" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14"/>
@@ -2232,10 +2244,10 @@
       <c r="O25" s="79"/>
     </row>
     <row r="26" spans="1:15" ht="97.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="105" t="s">
+      <c r="A26" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="116" t="s">
+      <c r="B26" s="118" t="s">
         <v>48</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -2260,13 +2272,13 @@
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
-      <c r="M26" s="102" t="s">
+      <c r="M26" s="104" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="106"/>
-      <c r="B27" s="117"/>
+      <c r="A27" s="108"/>
+      <c r="B27" s="119"/>
       <c r="C27" s="7" t="s">
         <v>5</v>
       </c>
@@ -2289,11 +2301,11 @@
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="103"/>
+      <c r="M27" s="105"/>
     </row>
     <row r="28" spans="1:15" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="106"/>
-      <c r="B28" s="117"/>
+      <c r="A28" s="108"/>
+      <c r="B28" s="119"/>
       <c r="C28" s="8" t="s">
         <v>6</v>
       </c>
@@ -2316,11 +2328,11 @@
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="103"/>
+      <c r="M28" s="105"/>
     </row>
     <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="106"/>
-      <c r="B29" s="117"/>
+      <c r="A29" s="108"/>
+      <c r="B29" s="119"/>
       <c r="C29" s="8" t="s">
         <v>39</v>
       </c>
@@ -2343,11 +2355,11 @@
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="103"/>
+      <c r="M29" s="105"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="106"/>
-      <c r="B30" s="117"/>
+      <c r="A30" s="108"/>
+      <c r="B30" s="119"/>
       <c r="C30" s="8" t="s">
         <v>7</v>
       </c>
@@ -2370,11 +2382,11 @@
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="103"/>
+      <c r="M30" s="105"/>
     </row>
     <row r="31" spans="1:15" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="106"/>
-      <c r="B31" s="117"/>
+      <c r="A31" s="108"/>
+      <c r="B31" s="119"/>
       <c r="C31" s="8" t="s">
         <v>40</v>
       </c>
@@ -2397,11 +2409,11 @@
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-      <c r="M31" s="103"/>
+      <c r="M31" s="105"/>
     </row>
     <row r="32" spans="1:15" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="106"/>
-      <c r="B32" s="117"/>
+      <c r="A32" s="108"/>
+      <c r="B32" s="119"/>
       <c r="C32" s="8" t="s">
         <v>8</v>
       </c>
@@ -2424,11 +2436,11 @@
       </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="103"/>
+      <c r="M32" s="105"/>
     </row>
     <row r="33" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="106"/>
-      <c r="B33" s="117"/>
+      <c r="A33" s="108"/>
+      <c r="B33" s="119"/>
       <c r="C33" s="8" t="s">
         <v>9</v>
       </c>
@@ -2451,11 +2463,11 @@
       </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-      <c r="M33" s="103"/>
+      <c r="M33" s="105"/>
     </row>
     <row r="34" spans="1:13" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="106"/>
-      <c r="B34" s="117"/>
+      <c r="A34" s="108"/>
+      <c r="B34" s="119"/>
       <c r="C34" s="8" t="s">
         <v>10</v>
       </c>
@@ -2478,11 +2490,11 @@
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
-      <c r="M34" s="103"/>
+      <c r="M34" s="105"/>
     </row>
     <row r="35" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="106"/>
-      <c r="B35" s="117"/>
+      <c r="A35" s="108"/>
+      <c r="B35" s="119"/>
       <c r="C35" s="8" t="s">
         <v>11</v>
       </c>
@@ -2505,11 +2517,11 @@
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-      <c r="M35" s="103"/>
+      <c r="M35" s="105"/>
     </row>
     <row r="36" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="106"/>
-      <c r="B36" s="117"/>
+      <c r="A36" s="108"/>
+      <c r="B36" s="119"/>
       <c r="C36" s="8" t="s">
         <v>12</v>
       </c>
@@ -2532,11 +2544,11 @@
       </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
-      <c r="M36" s="103"/>
+      <c r="M36" s="105"/>
     </row>
     <row r="37" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="106"/>
-      <c r="B37" s="117"/>
+      <c r="A37" s="108"/>
+      <c r="B37" s="119"/>
       <c r="C37" s="8" t="s">
         <v>13</v>
       </c>
@@ -2559,11 +2571,11 @@
       </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
-      <c r="M37" s="103"/>
+      <c r="M37" s="105"/>
     </row>
     <row r="38" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="106"/>
-      <c r="B38" s="117"/>
+      <c r="A38" s="108"/>
+      <c r="B38" s="119"/>
       <c r="C38" s="8" t="s">
         <v>41</v>
       </c>
@@ -2586,11 +2598,11 @@
       </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
-      <c r="M38" s="103"/>
+      <c r="M38" s="105"/>
     </row>
     <row r="39" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="106"/>
-      <c r="B39" s="117"/>
+      <c r="A39" s="108"/>
+      <c r="B39" s="119"/>
       <c r="C39" s="8" t="s">
         <v>42</v>
       </c>
@@ -2613,18 +2625,18 @@
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
-      <c r="M39" s="103"/>
+      <c r="M39" s="105"/>
     </row>
     <row r="40" spans="1:13" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="106"/>
-      <c r="B40" s="117"/>
-      <c r="C40" s="111" t="s">
+      <c r="A40" s="108"/>
+      <c r="B40" s="119"/>
+      <c r="C40" s="113" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="9">
         <v>32</v>
       </c>
-      <c r="E40" s="114" t="s">
+      <c r="E40" s="116" t="s">
         <v>15</v>
       </c>
       <c r="F40" s="13"/>
@@ -2642,16 +2654,16 @@
       </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
-      <c r="M40" s="103"/>
+      <c r="M40" s="105"/>
     </row>
     <row r="41" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="106"/>
-      <c r="B41" s="117"/>
-      <c r="C41" s="112"/>
+      <c r="A41" s="108"/>
+      <c r="B41" s="119"/>
+      <c r="C41" s="114"/>
       <c r="D41" s="10">
         <v>32</v>
       </c>
-      <c r="E41" s="115"/>
+      <c r="E41" s="117"/>
       <c r="F41" s="12"/>
       <c r="G41" s="1" t="s">
         <v>49</v>
@@ -2667,16 +2679,16 @@
       </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
-      <c r="M41" s="103"/>
+      <c r="M41" s="105"/>
     </row>
     <row r="42" spans="1:13" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="106"/>
-      <c r="B42" s="117"/>
-      <c r="C42" s="112"/>
+      <c r="A42" s="108"/>
+      <c r="B42" s="119"/>
+      <c r="C42" s="114"/>
       <c r="D42" s="10">
         <v>32</v>
       </c>
-      <c r="E42" s="114" t="s">
+      <c r="E42" s="116" t="s">
         <v>17</v>
       </c>
       <c r="F42" s="11"/>
@@ -2694,16 +2706,16 @@
       </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="103"/>
+      <c r="M42" s="105"/>
     </row>
     <row r="43" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="106"/>
-      <c r="B43" s="117"/>
-      <c r="C43" s="113"/>
+      <c r="A43" s="108"/>
+      <c r="B43" s="119"/>
+      <c r="C43" s="115"/>
       <c r="D43" s="10">
         <v>32</v>
       </c>
-      <c r="E43" s="115"/>
+      <c r="E43" s="117"/>
       <c r="F43" s="12"/>
       <c r="G43" s="1" t="s">
         <v>49</v>
@@ -2719,12 +2731,12 @@
       </c>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
-      <c r="M43" s="103"/>
+      <c r="M43" s="105"/>
     </row>
     <row r="44" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="106"/>
-      <c r="B44" s="117"/>
-      <c r="C44" s="111" t="s">
+      <c r="A44" s="108"/>
+      <c r="B44" s="119"/>
+      <c r="C44" s="113" t="s">
         <v>18</v>
       </c>
       <c r="D44" s="9">
@@ -2748,12 +2760,12 @@
       </c>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-      <c r="M44" s="103"/>
+      <c r="M44" s="105"/>
     </row>
     <row r="45" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="106"/>
-      <c r="B45" s="117"/>
-      <c r="C45" s="112"/>
+      <c r="A45" s="108"/>
+      <c r="B45" s="119"/>
+      <c r="C45" s="114"/>
       <c r="D45" s="10">
         <v>30</v>
       </c>
@@ -2775,12 +2787,12 @@
       </c>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
-      <c r="M45" s="103"/>
+      <c r="M45" s="105"/>
     </row>
     <row r="46" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="106"/>
-      <c r="B46" s="117"/>
-      <c r="C46" s="111" t="s">
+      <c r="A46" s="108"/>
+      <c r="B46" s="119"/>
+      <c r="C46" s="113" t="s">
         <v>19</v>
       </c>
       <c r="D46" s="9">
@@ -2804,12 +2816,12 @@
       </c>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
-      <c r="M46" s="103"/>
+      <c r="M46" s="105"/>
     </row>
     <row r="47" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="106"/>
-      <c r="B47" s="117"/>
-      <c r="C47" s="112"/>
+      <c r="A47" s="108"/>
+      <c r="B47" s="119"/>
+      <c r="C47" s="114"/>
       <c r="D47" s="10">
         <v>35</v>
       </c>
@@ -2831,11 +2843,11 @@
       </c>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-      <c r="M47" s="103"/>
+      <c r="M47" s="105"/>
     </row>
     <row r="48" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="106"/>
-      <c r="B48" s="117"/>
+      <c r="A48" s="108"/>
+      <c r="B48" s="119"/>
       <c r="C48" s="8" t="s">
         <v>16</v>
       </c>
@@ -2858,11 +2870,11 @@
       </c>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
-      <c r="M48" s="103"/>
+      <c r="M48" s="105"/>
     </row>
     <row r="49" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="106"/>
-      <c r="B49" s="117"/>
+      <c r="A49" s="108"/>
+      <c r="B49" s="119"/>
       <c r="C49" s="8" t="s">
         <v>45</v>
       </c>
@@ -2885,11 +2897,11 @@
       </c>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
-      <c r="M49" s="103"/>
+      <c r="M49" s="105"/>
     </row>
     <row r="50" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="107"/>
-      <c r="B50" s="118"/>
+      <c r="A50" s="109"/>
+      <c r="B50" s="120"/>
       <c r="C50" s="8" t="s">
         <v>46</v>
       </c>
@@ -2912,7 +2924,7 @@
       </c>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
-      <c r="M50" s="104"/>
+      <c r="M50" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -2940,10 +2952,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2952,8 +2964,9 @@
     <col min="3" max="3" width="27.77734375" customWidth="1"/>
     <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" style="64" customWidth="1"/>
+    <col min="8" max="8" width="5.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="91" customFormat="1" ht="18" x14ac:dyDescent="0.35">
@@ -2983,10 +2996,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="103" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="96" t="s">
         <v>107</v>
       </c>
       <c r="C4" s="80" t="s">
@@ -3085,7 +3098,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C18" s="123" t="s">
+      <c r="C18" s="125" t="s">
         <v>115</v>
       </c>
       <c r="D18" s="90" t="s">
@@ -3093,7 +3106,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C19" s="124"/>
+      <c r="C19" s="126"/>
       <c r="D19" s="90" t="s">
         <v>124</v>
       </c>
@@ -3104,16 +3117,16 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="97" t="s">
+      <c r="B21" s="96" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="99"/>
+      <c r="C21" s="98"/>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="97" t="s">
+      <c r="B22" s="96" t="s">
         <v>142</v>
       </c>
-      <c r="C22" s="100" t="s">
+      <c r="C22" s="99" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3123,10 +3136,10 @@
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="1:7" s="26" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="127" t="s">
+      <c r="A26" s="103" t="s">
         <v>138</v>
       </c>
-      <c r="B26" s="97" t="s">
+      <c r="B26" s="96" t="s">
         <v>140</v>
       </c>
       <c r="C26" s="81" t="s">
@@ -3348,56 +3361,56 @@
       </c>
       <c r="G48" s="71"/>
     </row>
-    <row r="49" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C49" s="61"/>
       <c r="D49" s="44" t="s">
         <v>69</v>
       </c>
       <c r="G49" s="71"/>
     </row>
-    <row r="50" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C50" s="61"/>
       <c r="D50" s="44" t="s">
         <v>70</v>
       </c>
       <c r="G50" s="71"/>
     </row>
-    <row r="51" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C51" s="61"/>
       <c r="D51" s="44" t="s">
         <v>71</v>
       </c>
       <c r="G51" s="71"/>
     </row>
-    <row r="52" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C52" s="61"/>
       <c r="D52" s="44" t="s">
         <v>72</v>
       </c>
       <c r="G52" s="71"/>
     </row>
-    <row r="53" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C53" s="61"/>
       <c r="D53" s="44" t="s">
         <v>73</v>
       </c>
       <c r="G53" s="71"/>
     </row>
-    <row r="54" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C54" s="61"/>
       <c r="D54" s="44" t="s">
         <v>74</v>
       </c>
       <c r="G54" s="71"/>
     </row>
-    <row r="55" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C55" s="62"/>
       <c r="D55" s="45" t="s">
         <v>67</v>
       </c>
       <c r="G55" s="71"/>
     </row>
-    <row r="56" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C56" s="47" t="s">
         <v>120</v>
       </c>
@@ -3406,14 +3419,14 @@
       </c>
       <c r="G56" s="71"/>
     </row>
-    <row r="57" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C57" s="48"/>
       <c r="D57" s="94" t="s">
         <v>78</v>
       </c>
       <c r="G57" s="71"/>
     </row>
-    <row r="58" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="93"/>
       <c r="D58" s="47" t="s">
         <v>133</v>
@@ -3424,12 +3437,14 @@
       <c r="F58" s="46">
         <v>4</v>
       </c>
-      <c r="G58" s="71"/>
-    </row>
-    <row r="59" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G58" s="46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C59" s="93"/>
       <c r="D59" s="48"/>
-      <c r="E59" s="46" t="s">
+      <c r="E59" s="94" t="s">
         <v>99</v>
       </c>
       <c r="F59" s="46" t="s">
@@ -3437,323 +3452,356 @@
       </c>
       <c r="G59" s="71"/>
     </row>
-    <row r="60" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C60" s="93"/>
-      <c r="D60" s="48"/>
-      <c r="E60" s="46" t="s">
+      <c r="D60" s="93"/>
+      <c r="E60" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="F60" s="46"/>
-      <c r="G60" s="96"/>
-    </row>
-    <row r="61" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F60" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="G60" s="128">
+        <v>17</v>
+      </c>
+      <c r="H60" s="46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C61" s="93"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="F61" s="46">
-        <v>1</v>
-      </c>
-      <c r="G61" s="71"/>
-    </row>
-    <row r="62" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D61" s="93"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="G61" s="128">
+        <v>13</v>
+      </c>
+      <c r="H61" s="46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C62" s="93"/>
       <c r="D62" s="48"/>
-      <c r="E62" s="46" t="s">
+      <c r="E62" s="95" t="s">
+        <v>131</v>
+      </c>
+      <c r="F62" s="46">
+        <v>1</v>
+      </c>
+      <c r="G62" s="46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="93"/>
+      <c r="D63" s="48"/>
+      <c r="E63" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="F62" s="46"/>
-      <c r="G62" s="71"/>
-    </row>
-    <row r="63" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C63" s="93"/>
-      <c r="D63" s="49"/>
-      <c r="E63" s="46" t="s">
+      <c r="F63" s="46"/>
+      <c r="G63" s="71"/>
+    </row>
+    <row r="64" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="93"/>
+      <c r="D64" s="49"/>
+      <c r="E64" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="F63" s="46">
+      <c r="F64" s="46">
         <v>1</v>
       </c>
-      <c r="G63" s="71"/>
-    </row>
-    <row r="64" spans="3:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="48"/>
-      <c r="D64" s="95" t="s">
-        <v>79</v>
-      </c>
-      <c r="G64" s="71"/>
+      <c r="G64" s="46" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="65" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C65" s="48"/>
-      <c r="D65" s="46" t="s">
+      <c r="D65" s="95" t="s">
+        <v>79</v>
+      </c>
+      <c r="G65" s="71"/>
+    </row>
+    <row r="66" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="48"/>
+      <c r="D66" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="G65" s="71"/>
-    </row>
-    <row r="66" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C66" s="49"/>
-      <c r="D66" s="46" t="s">
+      <c r="G66" s="71"/>
+    </row>
+    <row r="67" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="49"/>
+      <c r="D67" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="G66" s="71"/>
-    </row>
-    <row r="67" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C67" s="51" t="s">
+      <c r="G67" s="71"/>
+    </row>
+    <row r="68" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C68" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="D67" s="52" t="s">
+      <c r="D68" s="52" t="s">
         <v>82</v>
-      </c>
-      <c r="G67" s="71"/>
-    </row>
-    <row r="68" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C68" s="53"/>
-      <c r="D68" s="52" t="s">
-        <v>83</v>
       </c>
       <c r="G68" s="71"/>
     </row>
     <row r="69" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C69" s="53"/>
       <c r="D69" s="52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G69" s="71"/>
     </row>
     <row r="70" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C70" s="53"/>
       <c r="D70" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="G70" s="71"/>
+    </row>
+    <row r="71" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="53"/>
+      <c r="D71" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="G70" s="71"/>
-    </row>
-    <row r="71" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C71" s="54"/>
-      <c r="D71" s="52" t="s">
+      <c r="G71" s="71"/>
+    </row>
+    <row r="72" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C72" s="54"/>
+      <c r="D72" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="G71" s="71"/>
-    </row>
-    <row r="72" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C72" s="75" t="s">
+      <c r="G72" s="71"/>
+    </row>
+    <row r="73" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C73" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="D72" s="57" t="s">
+      <c r="D73" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="G72" s="71"/>
-    </row>
-    <row r="73" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C73" s="76"/>
-      <c r="D73" s="59" t="s">
+      <c r="G73" s="71"/>
+    </row>
+    <row r="74" spans="3:8" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C74" s="76"/>
+      <c r="D74" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="G73" s="71"/>
-    </row>
-    <row r="74" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C74" s="77"/>
-      <c r="D74" s="120" t="s">
-        <v>89</v>
-      </c>
-      <c r="E74" s="59" t="s">
-        <v>94</v>
-      </c>
-      <c r="F74" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="G74" s="72"/>
-      <c r="H74" s="72"/>
+      <c r="G74" s="71"/>
     </row>
     <row r="75" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C75" s="77"/>
-      <c r="D75" s="121"/>
-      <c r="E75" s="60"/>
+      <c r="D75" s="122" t="s">
+        <v>89</v>
+      </c>
+      <c r="E75" s="59" t="s">
+        <v>94</v>
+      </c>
       <c r="F75" s="58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G75" s="72"/>
       <c r="H75" s="72"/>
     </row>
     <row r="76" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C76" s="77"/>
-      <c r="D76" s="121"/>
-      <c r="E76" s="59" t="s">
-        <v>99</v>
-      </c>
+      <c r="D76" s="123"/>
+      <c r="E76" s="60"/>
       <c r="F76" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="G76" s="72">
-        <v>13</v>
-      </c>
-      <c r="H76" s="72" t="s">
-        <v>147</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="G76" s="72"/>
+      <c r="H76" s="72"/>
     </row>
     <row r="77" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C77" s="77"/>
-      <c r="D77" s="121"/>
-      <c r="E77" s="60"/>
+      <c r="D77" s="123"/>
+      <c r="E77" s="59" t="s">
+        <v>99</v>
+      </c>
       <c r="F77" s="58" t="s">
-        <v>93</v>
-      </c>
-      <c r="G77" s="72"/>
-      <c r="H77" s="72"/>
+        <v>92</v>
+      </c>
+      <c r="G77" s="72">
+        <v>13</v>
+      </c>
+      <c r="H77" s="72" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="78" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C78" s="77"/>
-      <c r="D78" s="121"/>
-      <c r="E78" s="59" t="s">
-        <v>98</v>
-      </c>
+      <c r="D78" s="123"/>
+      <c r="E78" s="60"/>
       <c r="F78" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="G78" s="72">
-        <v>22</v>
-      </c>
-      <c r="H78" s="126" t="s">
-        <v>147</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="G78" s="72"/>
+      <c r="H78" s="72"/>
     </row>
     <row r="79" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C79" s="77"/>
-      <c r="D79" s="121"/>
-      <c r="E79" s="60"/>
+      <c r="D79" s="123"/>
+      <c r="E79" s="59" t="s">
+        <v>98</v>
+      </c>
       <c r="F79" s="58" t="s">
-        <v>93</v>
-      </c>
-      <c r="G79" s="72"/>
-      <c r="H79" s="72"/>
+        <v>92</v>
+      </c>
+      <c r="G79" s="72">
+        <v>22</v>
+      </c>
+      <c r="H79" s="102" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="80" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C80" s="77"/>
-      <c r="D80" s="121"/>
-      <c r="E80" s="59" t="s">
-        <v>95</v>
-      </c>
+      <c r="D80" s="123"/>
+      <c r="E80" s="60"/>
       <c r="F80" s="58" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G80" s="72"/>
       <c r="H80" s="72"/>
     </row>
     <row r="81" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C81" s="77"/>
-      <c r="D81" s="121"/>
-      <c r="E81" s="60"/>
+      <c r="D81" s="123"/>
+      <c r="E81" s="59" t="s">
+        <v>95</v>
+      </c>
       <c r="F81" s="58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G81" s="72"/>
       <c r="H81" s="72"/>
     </row>
     <row r="82" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C82" s="77"/>
-      <c r="D82" s="121"/>
-      <c r="E82" s="59" t="s">
-        <v>96</v>
-      </c>
+      <c r="D82" s="123"/>
+      <c r="E82" s="60"/>
       <c r="F82" s="58" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G82" s="72"/>
       <c r="H82" s="72"/>
     </row>
     <row r="83" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C83" s="77"/>
-      <c r="D83" s="121"/>
-      <c r="E83" s="60"/>
+      <c r="D83" s="123"/>
+      <c r="E83" s="59" t="s">
+        <v>96</v>
+      </c>
       <c r="F83" s="58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G83" s="72"/>
       <c r="H83" s="72"/>
     </row>
     <row r="84" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C84" s="77"/>
-      <c r="D84" s="121"/>
-      <c r="E84" s="73" t="s">
-        <v>97</v>
-      </c>
+      <c r="D84" s="123"/>
+      <c r="E84" s="60"/>
       <c r="F84" s="58" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G84" s="72"/>
       <c r="H84" s="72"/>
     </row>
     <row r="85" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C85" s="77"/>
-      <c r="D85" s="122"/>
-      <c r="E85" s="60"/>
+      <c r="D85" s="123"/>
+      <c r="E85" s="73" t="s">
+        <v>97</v>
+      </c>
       <c r="F85" s="58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G85" s="72"/>
       <c r="H85" s="72"/>
     </row>
     <row r="86" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C86" s="77"/>
-      <c r="D86" s="60" t="s">
-        <v>102</v>
-      </c>
+      <c r="D86" s="124"/>
+      <c r="E86" s="60"/>
+      <c r="F86" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="G86" s="72"/>
+      <c r="H86" s="72"/>
     </row>
     <row r="87" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C87" s="77"/>
-      <c r="D87" s="57" t="s">
-        <v>90</v>
+      <c r="D87" s="60" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C88" s="77"/>
-      <c r="D88" s="59" t="s">
+      <c r="D88" s="57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C89" s="77"/>
+      <c r="D89" s="59" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="89" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C89" s="125" t="s">
+    <row r="90" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C90" s="127" t="s">
         <v>136</v>
       </c>
-      <c r="D89" s="98" t="s">
+      <c r="D90" s="97" t="s">
         <v>145</v>
       </c>
-      <c r="E89" s="101">
+      <c r="E90" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C90" s="125"/>
-      <c r="D90" s="98" t="s">
+      <c r="F90" s="101" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="91" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C91" s="127"/>
+      <c r="D91" s="97" t="s">
         <v>144</v>
       </c>
-      <c r="E90" s="101"/>
-    </row>
-    <row r="91" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C91" s="125"/>
-      <c r="D91" s="98"/>
-      <c r="E91" s="101"/>
+      <c r="E91" s="100"/>
+      <c r="F91" s="101"/>
     </row>
     <row r="92" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C92" s="125"/>
-      <c r="D92" s="98"/>
-      <c r="E92" s="101"/>
+      <c r="C92" s="127"/>
+      <c r="D92" s="97"/>
+      <c r="E92" s="100"/>
+      <c r="F92" s="101"/>
     </row>
     <row r="93" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C93" s="125"/>
-      <c r="D93" s="98"/>
-      <c r="E93" s="101"/>
+      <c r="C93" s="127"/>
+      <c r="D93" s="97"/>
+      <c r="E93" s="100"/>
+      <c r="F93" s="101"/>
     </row>
     <row r="94" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C94" s="125"/>
-      <c r="D94" s="98"/>
-      <c r="E94" s="101"/>
+      <c r="C94" s="127"/>
+      <c r="D94" s="97"/>
+      <c r="E94" s="100"/>
+      <c r="F94" s="101"/>
+    </row>
+    <row r="95" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C95" s="127"/>
+      <c r="D95" s="97"/>
+      <c r="E95" s="100"/>
+      <c r="F95" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D74:D85"/>
+    <mergeCell ref="D75:D86"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C89:C94"/>
+    <mergeCell ref="C90:C95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>